<commit_message>
Use a scanner in the Excel file for the detector offset test
</commit_message>
<xml_diff>
--- a/data/pretuning.xlsx
+++ b/data/pretuning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matteo\Università\Tesi\striptease\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564F0A3D-28E3-42B9-8292-76F32B006B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09D7BB2-743C-40A0-BAF9-8F51C8242DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="73">
   <si>
     <t>V1</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>3000;7000;5;[0,0,0,0];[4095,4095,4095,4095];5</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>LinearScanner</t>
+  </si>
+  <si>
+    <t>[0,0,0,0];[4095,4095,4095,4095];5</t>
   </si>
 </sst>
 </file>
@@ -570,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,9 +600,11 @@
     <col min="11" max="11" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -615,8 +626,11 @@
       <c r="L1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
         <v>55</v>
@@ -654,8 +668,14 @@
       <c r="M2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -695,8 +715,14 @@
       <c r="M3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,8 +762,14 @@
       <c r="M4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -777,8 +809,14 @@
       <c r="M5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -818,8 +856,14 @@
       <c r="M6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -859,8 +903,14 @@
       <c r="M7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>71</v>
+      </c>
+      <c r="O7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -900,8 +950,14 @@
       <c r="M8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -941,8 +997,14 @@
       <c r="M9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>71</v>
+      </c>
+      <c r="O9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -982,8 +1044,14 @@
       <c r="M10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>71</v>
+      </c>
+      <c r="O10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1023,8 +1091,14 @@
       <c r="M11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1064,8 +1138,14 @@
       <c r="M12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1105,8 +1185,14 @@
       <c r="M13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>71</v>
+      </c>
+      <c r="O13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1146,8 +1232,14 @@
       <c r="M14" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1187,8 +1279,14 @@
       <c r="M15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1228,8 +1326,14 @@
       <c r="M16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>71</v>
+      </c>
+      <c r="O16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1269,8 +1373,14 @@
       <c r="M17" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>71</v>
+      </c>
+      <c r="O17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1310,8 +1420,14 @@
       <c r="M18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1351,8 +1467,14 @@
       <c r="M19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1392,8 +1514,14 @@
       <c r="M20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>71</v>
+      </c>
+      <c r="O20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1433,8 +1561,14 @@
       <c r="M21" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>71</v>
+      </c>
+      <c r="O21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1474,8 +1608,14 @@
       <c r="M22" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>71</v>
+      </c>
+      <c r="O22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1515,8 +1655,14 @@
       <c r="M23" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>71</v>
+      </c>
+      <c r="O23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -1556,8 +1702,14 @@
       <c r="M24" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>71</v>
+      </c>
+      <c r="O24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -1597,8 +1749,14 @@
       <c r="M25" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>71</v>
+      </c>
+      <c r="O25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1638,8 +1796,14 @@
       <c r="M26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>71</v>
+      </c>
+      <c r="O26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1679,8 +1843,14 @@
       <c r="M27" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>71</v>
+      </c>
+      <c r="O27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1720,8 +1890,14 @@
       <c r="M28" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>71</v>
+      </c>
+      <c r="O28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1761,8 +1937,14 @@
       <c r="M29" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>71</v>
+      </c>
+      <c r="O29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -1802,8 +1984,14 @@
       <c r="M30" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>71</v>
+      </c>
+      <c r="O30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1843,8 +2031,14 @@
       <c r="M31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>71</v>
+      </c>
+      <c r="O31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -1884,8 +2078,14 @@
       <c r="M32" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>71</v>
+      </c>
+      <c r="O32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -1925,8 +2125,14 @@
       <c r="M33" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>71</v>
+      </c>
+      <c r="O33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -1966,8 +2172,14 @@
       <c r="M34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>71</v>
+      </c>
+      <c r="O34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -2007,8 +2219,14 @@
       <c r="M35" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>71</v>
+      </c>
+      <c r="O35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -2048,8 +2266,14 @@
       <c r="M36" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>71</v>
+      </c>
+      <c r="O36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -2089,8 +2313,14 @@
       <c r="M37" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>71</v>
+      </c>
+      <c r="O37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -2130,8 +2360,14 @@
       <c r="M38" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>71</v>
+      </c>
+      <c r="O38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -2171,8 +2407,14 @@
       <c r="M39" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>71</v>
+      </c>
+      <c r="O39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -2212,8 +2454,14 @@
       <c r="M40" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>71</v>
+      </c>
+      <c r="O40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -2253,8 +2501,14 @@
       <c r="M41" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>71</v>
+      </c>
+      <c r="O41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -2294,8 +2548,14 @@
       <c r="M42" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>71</v>
+      </c>
+      <c r="O42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -2335,8 +2595,14 @@
       <c r="M43" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>71</v>
+      </c>
+      <c r="O43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
@@ -2376,8 +2642,14 @@
       <c r="M44" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>71</v>
+      </c>
+      <c r="O44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -2417,8 +2689,14 @@
       <c r="M45" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>71</v>
+      </c>
+      <c r="O45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -2458,8 +2736,14 @@
       <c r="M46" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>71</v>
+      </c>
+      <c r="O46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
@@ -2499,8 +2783,14 @@
       <c r="M47" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>71</v>
+      </c>
+      <c r="O47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
@@ -2540,8 +2830,14 @@
       <c r="M48" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>71</v>
+      </c>
+      <c r="O48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
@@ -2581,8 +2877,14 @@
       <c r="M49" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>71</v>
+      </c>
+      <c r="O49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>46</v>
       </c>
@@ -2622,8 +2924,14 @@
       <c r="M50" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>71</v>
+      </c>
+      <c r="O50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
@@ -2663,8 +2971,14 @@
       <c r="M51" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" t="s">
+        <v>71</v>
+      </c>
+      <c r="O51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -2704,8 +3018,14 @@
       <c r="M52" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" t="s">
+        <v>71</v>
+      </c>
+      <c r="O52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
@@ -2745,8 +3065,14 @@
       <c r="M53" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53" t="s">
+        <v>71</v>
+      </c>
+      <c r="O53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
@@ -2786,8 +3112,14 @@
       <c r="M54" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54" t="s">
+        <v>71</v>
+      </c>
+      <c r="O54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
@@ -2827,8 +3159,14 @@
       <c r="M55" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55" t="s">
+        <v>71</v>
+      </c>
+      <c r="O55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
@@ -2868,8 +3206,14 @@
       <c r="M56" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56" t="s">
+        <v>71</v>
+      </c>
+      <c r="O56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
@@ -2909,8 +3253,14 @@
       <c r="M57" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57" t="s">
+        <v>71</v>
+      </c>
+      <c r="O57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
@@ -2949,6 +3299,12 @@
       </c>
       <c r="M58" t="s">
         <v>67</v>
+      </c>
+      <c r="N58" t="s">
+        <v>71</v>
+      </c>
+      <c r="O58" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>